<commit_message>
process scenes wo tags
</commit_message>
<xml_diff>
--- a/Projects/MARSUAE/Tests/Data/test_case_1.xlsx
+++ b/Projects/MARSUAE/Tests/Data/test_case_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,8 +15,8 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$N$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$52</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$N$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$127</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
@@ -34,17 +34,19 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$N$29</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$N$29</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">scif!$A$1:$N$18</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$A$1:$N$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">scif!$A$1:$N$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$18</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$N$14</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -550,24 +552,25 @@
   </sheetPr>
   <dimension ref="1:129"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C120" activeCellId="0" sqref="C120"/>
+      <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4861,23 +4864,24 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5606,29 +5610,31 @@
   </sheetPr>
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.9642857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8050,7 +8056,7 @@
         <v>36</v>
       </c>
       <c r="G34" s="10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>79</v>
@@ -8123,7 +8129,7 @@
         <v>13</v>
       </c>
       <c r="G35" s="10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>79</v>
@@ -8196,7 +8202,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>79</v>
@@ -8926,7 +8932,7 @@
         <v>2</v>
       </c>
       <c r="G46" s="9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>79</v>
@@ -8999,7 +9005,7 @@
         <v>3</v>
       </c>
       <c r="G47" s="9" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>79</v>
@@ -9072,7 +9078,7 @@
         <v>4</v>
       </c>
       <c r="G48" s="9" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>79</v>
@@ -9145,7 +9151,7 @@
         <v>5</v>
       </c>
       <c r="G49" s="9" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>79</v>
@@ -9218,7 +9224,7 @@
         <v>6</v>
       </c>
       <c r="G50" s="9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>79</v>
@@ -9291,7 +9297,7 @@
         <v>7</v>
       </c>
       <c r="G51" s="9" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H51" s="9" t="s">
         <v>79</v>
@@ -9364,7 +9370,7 @@
         <v>8</v>
       </c>
       <c r="G52" s="9" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>79</v>
@@ -9437,7 +9443,7 @@
         <v>9</v>
       </c>
       <c r="G53" s="9" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>79</v>
@@ -9510,7 +9516,7 @@
         <v>10</v>
       </c>
       <c r="G54" s="9" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>79</v>
@@ -9633,7 +9639,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N14"/>
+  <autoFilter ref="A1:N29"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -9652,13 +9658,14 @@
   </sheetPr>
   <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I137" activeCellId="0" sqref="I137"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B130" activeCellId="0" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>